<commit_message>
Customized section length / commented
</commit_message>
<xml_diff>
--- a/00.xlsx
+++ b/00.xlsx
@@ -424,27 +424,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>d4</t>
+          <t>c4</t>
         </is>
       </c>
       <c r="B1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>e4</t>
+          <t>d4</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>c4</t>
+          <t>e4</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -454,7 +454,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>d4</t>
+          <t>f4</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -474,7 +474,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>e4</t>
+          <t>c4</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -484,17 +484,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>d4</t>
+          <t>g3</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>c4</t>
+          <t>b3</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -504,7 +504,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>d4</t>
+          <t>c4</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -514,7 +514,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>e4</t>
+          <t>c5</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -524,7 +524,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>f4</t>
+          <t>g4</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -538,23 +538,23 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>d4</t>
+          <t>a4</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>c4</t>
+          <t>g4</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -564,7 +564,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>d4</t>
+          <t>c5</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -574,17 +574,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>e4</t>
+          <t>g4</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>e4</t>
+          <t>a4</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -594,7 +594,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>d4</t>
+          <t>c5</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -604,17 +604,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>d4</t>
+          <t>c5</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>g3</t>
+          <t>d5</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -624,37 +624,37 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>c4</t>
+          <t>e5</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>d4</t>
+          <t>d5</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>e4</t>
+          <t>c5</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>c4</t>
+          <t>a4</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -664,7 +664,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>d4</t>
+          <t>d5</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -674,37 +674,37 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>e4</t>
+          <t>c5</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>f4</t>
+          <t>a4</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>g4</t>
+          <t>d5</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>c4</t>
+          <t>c5</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -714,7 +714,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>c4</t>
+          <t>g4</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -724,7 +724,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>g4</t>
+          <t>e4</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -734,7 +734,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>f4</t>
+          <t>a4</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -744,7 +744,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>e4</t>
+          <t>g4</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -754,7 +754,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>g3</t>
+          <t>c5</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -764,17 +764,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>g3</t>
+          <t>g4</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>g4</t>
+          <t>a4</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -784,7 +784,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>g4</t>
+          <t>d4</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -794,11 +794,11 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>f4</t>
+          <t>d4</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
@@ -814,7 +814,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>c4</t>
+          <t>f4</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -824,11 +824,11 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>d4</t>
+          <t>g4</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42">
@@ -838,13 +838,13 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>d4</t>
+          <t>c4</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -854,17 +854,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>e4</t>
+          <t>g4</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>f4</t>
+          <t>g4</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -874,7 +874,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>e4</t>
+          <t>a4</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -884,17 +884,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>g3</t>
+          <t>d4</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>c4</t>
+          <t>d4</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -904,7 +904,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>d4</t>
+          <t>e4</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -914,7 +914,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>e4</t>
+          <t>c4</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -924,17 +924,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>c4</t>
+          <t>g3</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>g3</t>
+          <t>c4</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -944,17 +944,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>c4</t>
+          <t>d4</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>d4</t>
+          <t>e4</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -964,17 +964,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>e4</t>
+          <t>f4</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>f4</t>
+          <t>g4</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -984,7 +984,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>g4</t>
+          <t>c4</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -998,23 +998,23 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>c4</t>
+          <t>g3</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>g4</t>
+          <t>c4</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1024,17 +1024,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>g4</t>
+          <t>d4</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>f4</t>
+          <t>e4</t>
         </is>
       </c>
       <c r="B62" t="n">

</xml_diff>

<commit_message>
Fixed bug of bar counting
</commit_message>
<xml_diff>
--- a/00.xlsx
+++ b/00.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:B89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,17 +424,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>a4</t>
+          <t>g4</t>
         </is>
       </c>
       <c r="B1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>c5</t>
+          <t>g4</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -444,7 +444,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>c5</t>
+          <t>e4</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -454,7 +454,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>d5</t>
+          <t>a4</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -464,7 +464,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>e5</t>
+          <t>g4</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -474,7 +474,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>d5</t>
+          <t>c5</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -484,27 +484,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>c5</t>
+          <t>g4</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>a4</t>
+          <t>d4</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>d5</t>
+          <t>e4</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -514,117 +514,117 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>c5</t>
+          <t>d4</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>a4</t>
+          <t>d4</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>d5</t>
+          <t>g3</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>c5</t>
+          <t>c4</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>g4</t>
+          <t>d4</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>a4</t>
+          <t>e4</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>c5</t>
+          <t>d4</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>c5</t>
+          <t>e4</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>d5</t>
+          <t>f4</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>e5</t>
+          <t>e4</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>d5</t>
+          <t>g3</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>c5</t>
+          <t>c4</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -634,61 +634,61 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>a4</t>
+          <t>d4</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>d5</t>
+          <t>e4</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>c5</t>
+          <t>f4</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>g4</t>
+          <t>e4</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>e4</t>
+          <t>c4</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>a4</t>
+          <t>c4</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28">
@@ -698,33 +698,33 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>c5</t>
+          <t>f4</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>g4</t>
+          <t>e4</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>a4</t>
+          <t>g3</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -734,147 +734,147 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>c5</t>
+          <t>g3</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>c5</t>
+          <t>g4</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>d5</t>
+          <t>g4</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>e5</t>
+          <t>a4</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>d5</t>
+          <t>d4</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>c5</t>
+          <t>d4</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>g4</t>
+          <t>g3</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>a4</t>
+          <t>c4</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>c5</t>
+          <t>d4</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>c5</t>
+          <t>e4</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>d5</t>
+          <t>g3</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>e5</t>
+          <t>c4</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>d5</t>
+          <t>d4</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>c5</t>
+          <t>e4</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>g4</t>
+          <t>d4</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -884,41 +884,41 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>a4</t>
+          <t>e4</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>d4</t>
+          <t>f4</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>d4</t>
+          <t>g4</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>g3</t>
+          <t>c4</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51">
@@ -928,53 +928,53 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>d4</t>
+          <t>g4</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>e4</t>
+          <t>g4</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>d4</t>
+          <t>g4</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>c4</t>
+          <t>a4</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>d4</t>
+          <t>c5</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -984,60 +984,330 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>b3</t>
+          <t>c5</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>c4</t>
+          <t>d5</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>c5</t>
+          <t>e5</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>g4</t>
+          <t>d5</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>d4</t>
+          <t>c5</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
+          <t>a4</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>d5</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>c5</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>a4</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>d5</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>c5</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>g4</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
           <t>e4</t>
         </is>
       </c>
-      <c r="B62" t="n">
+      <c r="B69" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>a4</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>g4</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>c5</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>g4</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>e4</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>a4</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>g4</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>c5</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>g4</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>d4</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>e4</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>f4</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>g4</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>c4</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>c4</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>g3</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>b3</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>c4</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>c5</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>g4</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>